<commit_message>
Create PopupManager, minor fix
</commit_message>
<xml_diff>
--- a/Excel/GameSystem.xlsx
+++ b/Excel/GameSystem.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -488,6 +488,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>